<commit_message>
kernel loss is too bad
</commit_message>
<xml_diff>
--- a/output/LOSS.xlsx
+++ b/output/LOSS.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\2023\computional imaging\my_pbrt\output\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C26A7B57-70F6-4B7B-B324-B7BF8B2CCD39}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C347104E-E82B-458B-9007-A3898FE31EF1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="2808" yWindow="1716" windowWidth="17280" windowHeight="8880" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="3216" yWindow="2136" windowWidth="17280" windowHeight="8880" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="34" uniqueCount="24">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="39" uniqueCount="29">
   <si>
     <t>PBES</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -119,6 +119,26 @@
   </si>
   <si>
     <t>589(22s)</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>3.45（4）</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>742（35）</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>为何chamfer于kernel犯冲：事件数量！Kernel方法受事件数量影响严重，要保证输入的事件数量尽量一致</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>3.7022（5）</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>1965（49s)</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -444,10 +464,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:J7"/>
+  <dimension ref="A1:J10"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
-      <selection activeCell="F7" sqref="F7"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F11" sqref="F11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8" x14ac:dyDescent="0.25"/>
@@ -548,8 +568,20 @@
       <c r="A4" t="s">
         <v>6</v>
       </c>
+      <c r="B4" t="s">
+        <v>24</v>
+      </c>
+      <c r="C4" t="s">
+        <v>25</v>
+      </c>
       <c r="F4" t="s">
         <v>6</v>
+      </c>
+      <c r="G4" t="s">
+        <v>27</v>
+      </c>
+      <c r="H4" t="s">
+        <v>28</v>
       </c>
     </row>
     <row r="5" spans="1:10" x14ac:dyDescent="0.25">
@@ -574,6 +606,11 @@
       </c>
       <c r="F7" t="s">
         <v>8</v>
+      </c>
+    </row>
+    <row r="10" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="D10" t="s">
+        <v>26</v>
       </c>
     </row>
   </sheetData>

</xml_diff>